<commit_message>
introduces value with currency component for lksg backend fixtures and viewconfig
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/lksg/lksg.xlsx
+++ b/dataland-framework-toolbox/inputs/lksg/lksg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92928\Documents\Projects\Dataland\Dataland\dataland-framework-toolbox\inputs\lksg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\lksg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAB4AD4-272B-4E83-BD8B-B553DE47CE8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E28F16-7541-4204-9429-A50FB84224AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="530">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1657,13 +1657,10 @@
     <t>ISO2 Codes Multi-Select Dropdown</t>
   </si>
   <si>
-    <t>Currency</t>
-  </si>
-  <si>
     <t>119</t>
   </si>
   <si>
-    <t>Extended</t>
+    <t>LksgValueWithCurrencyComponent</t>
   </si>
 </sst>
 </file>
@@ -2157,29 +2154,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
   <dimension ref="A1:M203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E50" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="78.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="150.88671875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="87.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="39.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="23.109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.88671875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="18.44140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.36328125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="78.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="150.90625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="87.36328125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="39.6328125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="23.08984375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.90625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="12.36328125" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="4"/>
+    <col min="14" max="16384" width="9.08984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2220,7 +2217,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2243,7 +2240,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2263,7 +2260,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2283,7 +2280,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2309,7 +2306,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2329,7 +2326,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2355,7 +2352,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2375,7 +2372,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2404,7 +2401,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2421,13 +2418,10 @@
         <v>260</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>528</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2447,7 +2441,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2467,7 +2461,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2493,7 +2487,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2519,7 +2513,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2545,7 +2539,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2571,7 +2565,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2597,7 +2591,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2623,7 +2617,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2649,7 +2643,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2678,7 +2672,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2707,7 +2701,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -2733,7 +2727,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2759,7 +2753,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2782,7 +2776,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -2808,7 +2802,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -2834,7 +2828,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -2863,7 +2857,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -2889,7 +2883,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -2915,7 +2909,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -2941,7 +2935,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -2964,7 +2958,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -2990,7 +2984,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -3016,7 +3010,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -3042,7 +3036,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -3068,7 +3062,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -3094,7 +3088,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -3126,7 +3120,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -3155,7 +3149,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -3181,7 +3175,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -3207,7 +3201,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -3233,7 +3227,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -3259,7 +3253,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -3285,7 +3279,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -3311,7 +3305,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -3334,7 +3328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -3357,7 +3351,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -3383,7 +3377,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -3406,7 +3400,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -3429,7 +3423,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -3455,7 +3449,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -3478,7 +3472,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -3501,7 +3495,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -3521,7 +3515,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -3541,7 +3535,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -3561,7 +3555,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -3581,7 +3575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -3601,7 +3595,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -3630,7 +3624,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -3656,7 +3650,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -3682,7 +3676,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -3702,7 +3696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -3728,7 +3722,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -3748,7 +3742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -3774,7 +3768,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -3794,7 +3788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -3820,7 +3814,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -3840,7 +3834,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -3866,7 +3860,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -3892,7 +3886,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -3918,7 +3912,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -3944,7 +3938,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -3970,7 +3964,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -3990,7 +3984,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -4016,7 +4010,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -4042,7 +4036,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -4068,7 +4062,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -4097,7 +4091,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -4123,7 +4117,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -4152,7 +4146,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -4181,7 +4175,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -4207,7 +4201,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -4227,7 +4221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -4253,7 +4247,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -4273,7 +4267,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -4299,7 +4293,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -4325,7 +4319,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -4351,7 +4345,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -4377,7 +4371,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -4406,7 +4400,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -4435,7 +4429,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -4464,7 +4458,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -4490,7 +4484,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -4510,7 +4504,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -4530,7 +4524,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -4559,7 +4553,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -4588,7 +4582,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -4614,7 +4608,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -4640,7 +4634,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -4666,7 +4660,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -4695,7 +4689,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -4721,7 +4715,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -4741,7 +4735,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -4761,7 +4755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -4781,7 +4775,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -4810,7 +4804,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" s="4">
         <v>105</v>
       </c>
@@ -4839,7 +4833,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" s="4">
         <v>106</v>
       </c>
@@ -4868,7 +4862,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -4897,7 +4891,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" s="4">
         <v>108</v>
       </c>
@@ -4923,7 +4917,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -4943,7 +4937,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -4963,7 +4957,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" s="4">
         <v>111</v>
       </c>
@@ -4989,7 +4983,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" s="4">
         <v>112</v>
       </c>
@@ -5009,7 +5003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="4">
         <v>113</v>
       </c>
@@ -5035,7 +5029,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" s="4">
         <v>114</v>
       </c>
@@ -5061,7 +5055,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" s="4">
         <v>115</v>
       </c>
@@ -5090,7 +5084,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="4">
         <v>116</v>
       </c>
@@ -5119,7 +5113,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="4">
         <v>117</v>
       </c>
@@ -5148,7 +5142,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="4">
         <v>118</v>
       </c>
@@ -5174,7 +5168,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" s="4">
         <v>119</v>
       </c>
@@ -5194,7 +5188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" s="4">
         <v>120</v>
       </c>
@@ -5214,13 +5208,13 @@
         <v>20</v>
       </c>
       <c r="K121" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L121" s="4" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" s="4">
         <v>121</v>
       </c>
@@ -5240,13 +5234,13 @@
         <v>20</v>
       </c>
       <c r="K122" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L122" s="4" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" s="4">
         <v>122</v>
       </c>
@@ -5266,13 +5260,13 @@
         <v>20</v>
       </c>
       <c r="K123" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L123" s="4" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" s="4">
         <v>123</v>
       </c>
@@ -5295,13 +5289,13 @@
         <v>22</v>
       </c>
       <c r="K124" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L124" s="4" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" s="4">
         <v>124</v>
       </c>
@@ -5321,13 +5315,13 @@
         <v>20</v>
       </c>
       <c r="K125" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L125" s="4" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="4">
         <v>125</v>
       </c>
@@ -5350,13 +5344,13 @@
         <v>22</v>
       </c>
       <c r="K126" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L126" s="4" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" s="4">
         <v>126</v>
       </c>
@@ -5379,13 +5373,13 @@
         <v>22</v>
       </c>
       <c r="K127" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L127" s="4" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" s="4">
         <v>127</v>
       </c>
@@ -5411,7 +5405,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A129" s="4">
         <v>128</v>
       </c>
@@ -5431,7 +5425,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A130" s="4">
         <v>129</v>
       </c>
@@ -5457,7 +5451,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A131" s="4">
         <v>130</v>
       </c>
@@ -5483,7 +5477,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A132" s="4">
         <v>131</v>
       </c>
@@ -5509,7 +5503,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A133" s="4">
         <v>132</v>
       </c>
@@ -5535,7 +5529,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A134" s="4">
         <v>133</v>
       </c>
@@ -5561,7 +5555,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A135" s="4">
         <v>134</v>
       </c>
@@ -5590,7 +5584,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" s="4">
         <v>135</v>
       </c>
@@ -5619,7 +5613,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A137" s="4">
         <v>136</v>
       </c>
@@ -5639,7 +5633,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A138" s="4">
         <v>137</v>
       </c>
@@ -5665,7 +5659,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A139" s="4">
         <v>138</v>
       </c>
@@ -5691,7 +5685,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" s="4">
         <v>139</v>
       </c>
@@ -5720,7 +5714,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A141" s="4">
         <v>140</v>
       </c>
@@ -5749,7 +5743,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A142" s="4">
         <v>141</v>
       </c>
@@ -5769,7 +5763,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A143" s="4">
         <v>142</v>
       </c>
@@ -5795,7 +5789,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A144" s="4">
         <v>143</v>
       </c>
@@ -5824,7 +5818,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A145" s="4">
         <v>144</v>
       </c>
@@ -5853,7 +5847,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A146" s="4">
         <v>145</v>
       </c>
@@ -5873,7 +5867,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A147" s="4">
         <v>146</v>
       </c>
@@ -5899,7 +5893,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" s="4">
         <v>147</v>
       </c>
@@ -5928,7 +5922,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A149" s="4">
         <v>148</v>
       </c>
@@ -5957,7 +5951,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" s="4">
         <v>149</v>
       </c>
@@ -5977,7 +5971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A151" s="4">
         <v>150</v>
       </c>
@@ -6003,7 +5997,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" s="4">
         <v>151</v>
       </c>
@@ -6029,7 +6023,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A153" s="4">
         <v>152</v>
       </c>
@@ -6058,7 +6052,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" s="4">
         <v>153</v>
       </c>
@@ -6087,7 +6081,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A155" s="4">
         <v>154</v>
       </c>
@@ -6113,7 +6107,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" s="4">
         <v>155</v>
       </c>
@@ -6136,7 +6130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A157" s="4">
         <v>156</v>
       </c>
@@ -6162,7 +6156,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" s="4">
         <v>157</v>
       </c>
@@ -6182,7 +6176,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A159" s="4">
         <v>158</v>
       </c>
@@ -6208,7 +6202,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" s="4">
         <v>159</v>
       </c>
@@ -6228,7 +6222,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A161" s="4">
         <v>160</v>
       </c>
@@ -6257,7 +6251,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A162" s="4">
         <v>161</v>
       </c>
@@ -6283,7 +6277,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A163" s="4">
         <v>162</v>
       </c>
@@ -6312,7 +6306,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A164" s="4">
         <v>163</v>
       </c>
@@ -6341,7 +6335,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A165" s="4">
         <v>164</v>
       </c>
@@ -6367,7 +6361,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A166" s="4">
         <v>165</v>
       </c>
@@ -6387,7 +6381,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A167" s="4">
         <v>166</v>
       </c>
@@ -6407,7 +6401,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A168" s="4">
         <v>167</v>
       </c>
@@ -6433,7 +6427,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A169" s="4">
         <v>168</v>
       </c>
@@ -6462,7 +6456,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A170" s="4">
         <v>169</v>
       </c>
@@ -6491,7 +6485,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A171" s="4">
         <v>170</v>
       </c>
@@ -6517,7 +6511,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A172" s="4">
         <v>171</v>
       </c>
@@ -6546,7 +6540,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A173" s="4">
         <v>172</v>
       </c>
@@ -6575,7 +6569,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A174" s="4">
         <v>173</v>
       </c>
@@ -6601,7 +6595,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A175" s="4">
         <v>174</v>
       </c>
@@ -6621,7 +6615,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A176" s="4">
         <v>175</v>
       </c>
@@ -6647,7 +6641,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A177" s="4">
         <v>176</v>
       </c>
@@ -6673,7 +6667,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A178" s="4">
         <v>177</v>
       </c>
@@ -6699,7 +6693,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A179" s="4">
         <v>178</v>
       </c>
@@ -6725,7 +6719,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A180" s="4">
         <v>179</v>
       </c>
@@ -6751,7 +6745,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A181" s="4">
         <v>180</v>
       </c>
@@ -6777,7 +6771,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A182" s="4">
         <v>181</v>
       </c>
@@ -6806,7 +6800,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A183" s="4">
         <v>182</v>
       </c>
@@ -6835,7 +6829,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A184" s="4">
         <v>183</v>
       </c>
@@ -6861,7 +6855,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A185" s="4">
         <v>184</v>
       </c>
@@ -6881,7 +6875,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A186" s="4">
         <v>185</v>
       </c>
@@ -6907,7 +6901,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A187" s="4">
         <v>186</v>
       </c>
@@ -6933,7 +6927,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A188" s="4">
         <v>187</v>
       </c>
@@ -6959,7 +6953,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A189" s="4">
         <v>188</v>
       </c>
@@ -6985,7 +6979,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A190" s="4">
         <v>189</v>
       </c>
@@ -7011,7 +7005,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A191" s="4">
         <v>190</v>
       </c>
@@ -7040,7 +7034,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A192" s="4">
         <v>191</v>
       </c>
@@ -7066,7 +7060,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A193" s="4">
         <v>192</v>
       </c>
@@ -7086,7 +7080,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="194" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A194" s="4">
         <v>193</v>
       </c>
@@ -7112,7 +7106,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A195" s="4">
         <v>194</v>
       </c>
@@ -7138,7 +7132,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" s="4">
         <v>195</v>
       </c>
@@ -7164,7 +7158,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A197" s="4">
         <v>196</v>
       </c>
@@ -7190,7 +7184,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" s="4">
         <v>197</v>
       </c>
@@ -7219,7 +7213,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A199" s="4">
         <v>198</v>
       </c>
@@ -7245,7 +7239,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" s="4">
         <v>199</v>
       </c>
@@ -7265,7 +7259,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A201" s="4">
         <v>200</v>
       </c>
@@ -7291,7 +7285,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" s="4">
         <v>201</v>
       </c>
@@ -7320,7 +7314,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A203" s="9">
         <v>202</v>
       </c>
@@ -7360,15 +7354,15 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>471</v>
       </c>
@@ -7382,7 +7376,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>475</v>
       </c>
@@ -7396,7 +7390,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>478</v>
       </c>
@@ -7410,7 +7404,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>482</v>
       </c>
@@ -7424,7 +7418,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>486</v>
       </c>
@@ -7438,7 +7432,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>489</v>
       </c>
@@ -7452,7 +7446,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>492</v>
       </c>
@@ -7466,7 +7460,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>470</v>
       </c>
@@ -7480,7 +7474,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>497</v>
       </c>
@@ -7494,7 +7488,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>500</v>
       </c>
@@ -7508,7 +7502,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>503</v>
       </c>
@@ -7522,7 +7516,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>506</v>
       </c>
@@ -7536,7 +7530,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>509</v>
       </c>
@@ -7550,7 +7544,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
working capital now has a currency
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/lksg/lksg.xlsx
+++ b/dataland-framework-toolbox/inputs/lksg/lksg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\lksg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E28F16-7541-4204-9429-A50FB84224AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2393CBEC-24EB-4BD3-ACDD-7D4E9D6E881C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
@@ -2154,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
   <dimension ref="A1:M203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F11" sqref="E11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2438,7 +2438,7 @@
         <v>261</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>19</v>
+        <v>529</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
regenerates backendOpenApi.json, fake fixtures and updates excel
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/lksg/lksg.xlsx
+++ b/dataland-framework-toolbox/inputs/lksg/lksg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\Dataland\dataland-framework-toolbox\inputs\lksg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d92048\IdeaProjects\Dataland5\dataland-framework-toolbox\inputs\lksg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB582CBD-E321-4C81-B1B9-49DA82D9B6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938BC668-D21E-4DC6-AF41-72797EC62505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EA21DF-A91B-4C8A-A36C-EACA4F178F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="559">
   <si>
     <t>Field Identifier</t>
   </si>
@@ -1405,9 +1405,6 @@
     <t>Percentage</t>
   </si>
   <si>
-    <t>LkSG - risk Positions</t>
-  </si>
-  <si>
     <t>Multi-Select Dropdown</t>
   </si>
   <si>
@@ -1748,6 +1745,9 @@
   </si>
   <si>
     <t>198</t>
+  </si>
+  <si>
+    <t>LkSG Risk Position MultiSelect Component</t>
   </si>
 </sst>
 </file>
@@ -2247,8 +2247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBCA27A-793A-4293-9394-36A2BE726731}">
   <dimension ref="A1:M202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2330,7 +2330,7 @@
         <v>16</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -2396,7 +2396,7 @@
         <v>3</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -2416,7 +2416,7 @@
         <v>246</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -2439,7 +2439,7 @@
         <v>19</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>22</v>
@@ -2485,13 +2485,13 @@
         <v>17</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -2511,7 +2511,7 @@
         <v>250</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -2531,7 +2531,7 @@
         <v>251</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
@@ -2577,7 +2577,7 @@
         <v>11</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -2603,7 +2603,7 @@
         <v>11</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -2623,13 +2623,13 @@
         <v>255</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>44</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -2655,7 +2655,7 @@
         <v>11</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
@@ -2672,16 +2672,16 @@
         <v>59</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
@@ -2701,13 +2701,13 @@
         <v>257</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
@@ -2730,13 +2730,13 @@
         <v>17</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K19" s="7">
         <v>11</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
@@ -2756,16 +2756,16 @@
         <v>259</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K20" s="7">
         <v>11</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -2785,13 +2785,13 @@
         <v>260</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K21" s="7">
         <v>11</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -2805,19 +2805,19 @@
         <v>27</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>261</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K22" s="7">
         <v>11</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
@@ -2863,10 +2863,10 @@
         <v>20</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -2889,10 +2889,10 @@
         <v>20</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
@@ -2912,16 +2912,14 @@
         <v>265</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>444</v>
-      </c>
+        <v>558</v>
+      </c>
+      <c r="H26" s="9"/>
       <c r="K26" s="7" t="s">
         <v>441</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
@@ -2947,7 +2945,7 @@
         <v>441</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
@@ -2970,10 +2968,10 @@
         <v>442</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
@@ -2996,10 +2994,10 @@
         <v>20</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
@@ -3045,10 +3043,10 @@
         <v>20</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
@@ -3071,10 +3069,10 @@
         <v>20</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
@@ -3097,10 +3095,10 @@
         <v>20</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
@@ -3123,10 +3121,10 @@
         <v>20</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
@@ -3149,10 +3147,10 @@
         <v>20</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
@@ -3175,16 +3173,16 @@
         <v>19</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>22</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
@@ -3204,16 +3202,14 @@
         <v>276</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>444</v>
-      </c>
+        <v>558</v>
+      </c>
+      <c r="H37" s="9"/>
       <c r="K37" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
@@ -3236,10 +3232,10 @@
         <v>442</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
@@ -3262,10 +3258,10 @@
         <v>20</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
@@ -3288,10 +3284,10 @@
         <v>442</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
@@ -3314,10 +3310,10 @@
         <v>20</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
@@ -3340,10 +3336,10 @@
         <v>20</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
@@ -3366,10 +3362,10 @@
         <v>20</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
@@ -3438,10 +3434,10 @@
         <v>20</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
@@ -3510,10 +3506,10 @@
         <v>442</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
@@ -3679,16 +3675,14 @@
         <v>296</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="H57" s="9" t="s">
-        <v>444</v>
-      </c>
+        <v>558</v>
+      </c>
+      <c r="H57" s="9"/>
       <c r="K57" s="7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
@@ -3711,10 +3705,10 @@
         <v>20</v>
       </c>
       <c r="K58" s="7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
@@ -3737,10 +3731,10 @@
         <v>442</v>
       </c>
       <c r="K59" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
@@ -3780,13 +3774,13 @@
         <v>300</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K61" s="7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
@@ -3826,13 +3820,13 @@
         <v>302</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K63" s="7" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.35">
@@ -3872,13 +3866,13 @@
         <v>302</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K65" s="7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
@@ -3921,10 +3915,10 @@
         <v>20</v>
       </c>
       <c r="K67" s="7" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.35">
@@ -3947,10 +3941,10 @@
         <v>20</v>
       </c>
       <c r="K68" s="7" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.35">
@@ -3973,10 +3967,10 @@
         <v>20</v>
       </c>
       <c r="K69" s="7" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.35">
@@ -3999,10 +3993,10 @@
         <v>20</v>
       </c>
       <c r="K70" s="7" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.35">
@@ -4025,10 +4019,10 @@
         <v>442</v>
       </c>
       <c r="K71" s="7" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
@@ -4071,10 +4065,10 @@
         <v>20</v>
       </c>
       <c r="K73" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.35">
@@ -4097,10 +4091,10 @@
         <v>20</v>
       </c>
       <c r="K74" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.35">
@@ -4123,10 +4117,10 @@
         <v>20</v>
       </c>
       <c r="K75" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.35">
@@ -4152,10 +4146,10 @@
         <v>22</v>
       </c>
       <c r="K76" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.35">
@@ -4178,10 +4172,10 @@
         <v>20</v>
       </c>
       <c r="K77" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.35">
@@ -4207,10 +4201,10 @@
         <v>22</v>
       </c>
       <c r="K78" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.35">
@@ -4236,10 +4230,10 @@
         <v>22</v>
       </c>
       <c r="K79" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
@@ -4262,10 +4256,10 @@
         <v>442</v>
       </c>
       <c r="K80" s="7" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.35">
@@ -4308,10 +4302,10 @@
         <v>442</v>
       </c>
       <c r="K82" s="7" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.35">
@@ -4354,10 +4348,10 @@
         <v>20</v>
       </c>
       <c r="K84" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L84" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.35">
@@ -4380,10 +4374,10 @@
         <v>20</v>
       </c>
       <c r="K85" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.35">
@@ -4406,10 +4400,10 @@
         <v>20</v>
       </c>
       <c r="K86" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L86" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.35">
@@ -4432,10 +4426,10 @@
         <v>20</v>
       </c>
       <c r="K87" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L87" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.35">
@@ -4461,10 +4455,10 @@
         <v>22</v>
       </c>
       <c r="K88" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L88" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.35">
@@ -4490,10 +4484,10 @@
         <v>22</v>
       </c>
       <c r="K89" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L89" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.35">
@@ -4519,10 +4513,10 @@
         <v>22</v>
       </c>
       <c r="K90" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L90" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.35">
@@ -4542,13 +4536,13 @@
         <v>327</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K91" s="7" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L91" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.35">
@@ -4614,10 +4608,10 @@
         <v>22</v>
       </c>
       <c r="K94" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L94" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.35">
@@ -4643,10 +4637,10 @@
         <v>22</v>
       </c>
       <c r="K95" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L95" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.35">
@@ -4669,10 +4663,10 @@
         <v>20</v>
       </c>
       <c r="K96" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L96" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.35">
@@ -4692,13 +4686,13 @@
         <v>333</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K97" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L97" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.35">
@@ -4718,13 +4712,13 @@
         <v>334</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K98" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L98" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.35">
@@ -4750,10 +4744,10 @@
         <v>22</v>
       </c>
       <c r="K99" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L99" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.35">
@@ -4776,10 +4770,10 @@
         <v>442</v>
       </c>
       <c r="K100" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L100" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.35">
@@ -4865,10 +4859,10 @@
         <v>22</v>
       </c>
       <c r="K104" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L104" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.35">
@@ -4894,10 +4888,10 @@
         <v>22</v>
       </c>
       <c r="K105" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L105" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.35">
@@ -4923,10 +4917,10 @@
         <v>22</v>
       </c>
       <c r="K106" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L106" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.35">
@@ -4952,10 +4946,10 @@
         <v>22</v>
       </c>
       <c r="K107" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L107" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.35">
@@ -4978,10 +4972,10 @@
         <v>442</v>
       </c>
       <c r="K108" s="7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L108" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.35">
@@ -5044,10 +5038,10 @@
         <v>443</v>
       </c>
       <c r="K111" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L111" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.35">
@@ -5090,10 +5084,10 @@
         <v>20</v>
       </c>
       <c r="K113" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L113" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.35">
@@ -5116,10 +5110,10 @@
         <v>20</v>
       </c>
       <c r="K114" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L114" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.35">
@@ -5145,10 +5139,10 @@
         <v>22</v>
       </c>
       <c r="K115" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L115" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.35">
@@ -5174,10 +5168,10 @@
         <v>22</v>
       </c>
       <c r="K116" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L116" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.35">
@@ -5203,10 +5197,10 @@
         <v>22</v>
       </c>
       <c r="K117" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L117" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.35">
@@ -5229,10 +5223,10 @@
         <v>442</v>
       </c>
       <c r="K118" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L118" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.35">
@@ -5275,10 +5269,10 @@
         <v>20</v>
       </c>
       <c r="K120" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L120" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.35">
@@ -5301,10 +5295,10 @@
         <v>20</v>
       </c>
       <c r="K121" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L121" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.35">
@@ -5327,10 +5321,10 @@
         <v>20</v>
       </c>
       <c r="K122" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L122" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.35">
@@ -5356,10 +5350,10 @@
         <v>22</v>
       </c>
       <c r="K123" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L123" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.35">
@@ -5382,10 +5376,10 @@
         <v>20</v>
       </c>
       <c r="K124" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L124" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.35">
@@ -5411,10 +5405,10 @@
         <v>22</v>
       </c>
       <c r="K125" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L125" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.35">
@@ -5440,10 +5434,10 @@
         <v>22</v>
       </c>
       <c r="K126" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L126" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.35">
@@ -5466,10 +5460,10 @@
         <v>442</v>
       </c>
       <c r="K127" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L127" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.35">
@@ -5512,10 +5506,10 @@
         <v>20</v>
       </c>
       <c r="K129" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L129" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.35">
@@ -5538,10 +5532,10 @@
         <v>20</v>
       </c>
       <c r="K130" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L130" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.35">
@@ -5564,10 +5558,10 @@
         <v>20</v>
       </c>
       <c r="K131" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L131" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.35">
@@ -5590,10 +5584,10 @@
         <v>20</v>
       </c>
       <c r="K132" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L132" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.35">
@@ -5616,10 +5610,10 @@
         <v>20</v>
       </c>
       <c r="K133" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L133" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.35">
@@ -5645,10 +5639,10 @@
         <v>22</v>
       </c>
       <c r="K134" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L134" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.35">
@@ -5674,10 +5668,10 @@
         <v>22</v>
       </c>
       <c r="K135" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L135" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.35">
@@ -5720,10 +5714,10 @@
         <v>20</v>
       </c>
       <c r="K137" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L137" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.35">
@@ -5746,10 +5740,10 @@
         <v>20</v>
       </c>
       <c r="K138" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L138" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.35">
@@ -5775,10 +5769,10 @@
         <v>22</v>
       </c>
       <c r="K139" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L139" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.35">
@@ -5804,10 +5798,10 @@
         <v>22</v>
       </c>
       <c r="K140" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L140" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.35">
@@ -5850,10 +5844,10 @@
         <v>20</v>
       </c>
       <c r="K142" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L142" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.35">
@@ -5879,10 +5873,10 @@
         <v>22</v>
       </c>
       <c r="K143" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L143" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.35">
@@ -5908,10 +5902,10 @@
         <v>22</v>
       </c>
       <c r="K144" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L144" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.35">
@@ -5954,10 +5948,10 @@
         <v>20</v>
       </c>
       <c r="K146" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L146" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.35">
@@ -5983,10 +5977,10 @@
         <v>22</v>
       </c>
       <c r="K147" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L147" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.35">
@@ -6012,10 +6006,10 @@
         <v>22</v>
       </c>
       <c r="K148" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L148" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.35">
@@ -6058,10 +6052,10 @@
         <v>20</v>
       </c>
       <c r="K150" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L150" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.35">
@@ -6084,10 +6078,10 @@
         <v>442</v>
       </c>
       <c r="K151" s="7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L151" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.35">
@@ -6113,10 +6107,10 @@
         <v>22</v>
       </c>
       <c r="K152" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L152" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.35">
@@ -6142,10 +6136,10 @@
         <v>22</v>
       </c>
       <c r="K153" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L153" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.35">
@@ -6168,10 +6162,10 @@
         <v>20</v>
       </c>
       <c r="K154" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L154" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.35">
@@ -6217,10 +6211,10 @@
         <v>442</v>
       </c>
       <c r="K156" s="7" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="L156" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.35">
@@ -6263,10 +6257,10 @@
         <v>442</v>
       </c>
       <c r="K158" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L158" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.35">
@@ -6312,10 +6306,10 @@
         <v>22</v>
       </c>
       <c r="K160" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L160" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.35">
@@ -6338,10 +6332,10 @@
         <v>20</v>
       </c>
       <c r="K161" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L161" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.35">
@@ -6367,10 +6361,10 @@
         <v>22</v>
       </c>
       <c r="K162" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L162" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.35">
@@ -6396,10 +6390,10 @@
         <v>22</v>
       </c>
       <c r="K163" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L163" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.35">
@@ -6422,10 +6416,10 @@
         <v>442</v>
       </c>
       <c r="K164" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="L164" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.35">
@@ -6488,10 +6482,10 @@
         <v>20</v>
       </c>
       <c r="K167" s="7" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="L167" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.35">
@@ -6517,10 +6511,10 @@
         <v>22</v>
       </c>
       <c r="K168" s="7" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L168" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.35">
@@ -6546,10 +6540,10 @@
         <v>22</v>
       </c>
       <c r="K169" s="7" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L169" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.35">
@@ -6569,13 +6563,13 @@
         <v>402</v>
       </c>
       <c r="G170" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K170" s="7" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L170" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.35">
@@ -6595,16 +6589,16 @@
         <v>403</v>
       </c>
       <c r="G171" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J171" s="9" t="s">
         <v>22</v>
       </c>
       <c r="K171" s="7" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L171" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.35">
@@ -6630,10 +6624,10 @@
         <v>22</v>
       </c>
       <c r="K172" s="7" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L172" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.35">
@@ -6653,13 +6647,13 @@
         <v>405</v>
       </c>
       <c r="G173" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K173" s="7" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L173" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.35">
@@ -6702,10 +6696,10 @@
         <v>20</v>
       </c>
       <c r="K175" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L175" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.35">
@@ -6728,10 +6722,10 @@
         <v>20</v>
       </c>
       <c r="K176" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L176" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.35">
@@ -6754,10 +6748,10 @@
         <v>20</v>
       </c>
       <c r="K177" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L177" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.35">
@@ -6780,10 +6774,10 @@
         <v>20</v>
       </c>
       <c r="K178" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L178" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.35">
@@ -6806,10 +6800,10 @@
         <v>20</v>
       </c>
       <c r="K179" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L179" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.35">
@@ -6832,10 +6826,10 @@
         <v>20</v>
       </c>
       <c r="K180" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L180" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.35">
@@ -6861,10 +6855,10 @@
         <v>22</v>
       </c>
       <c r="K181" s="7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L181" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.35">
@@ -6890,10 +6884,10 @@
         <v>22</v>
       </c>
       <c r="K182" s="7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L182" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.35">
@@ -6916,10 +6910,10 @@
         <v>442</v>
       </c>
       <c r="K183" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L183" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.35">
@@ -6962,10 +6956,10 @@
         <v>442</v>
       </c>
       <c r="K185" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L185" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.35">
@@ -6988,10 +6982,10 @@
         <v>20</v>
       </c>
       <c r="K186" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L186" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.35">
@@ -7014,10 +7008,10 @@
         <v>20</v>
       </c>
       <c r="K187" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L187" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.35">
@@ -7040,10 +7034,10 @@
         <v>20</v>
       </c>
       <c r="K188" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L188" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.35">
@@ -7066,10 +7060,10 @@
         <v>20</v>
       </c>
       <c r="K189" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L189" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.35">
@@ -7095,10 +7089,10 @@
         <v>22</v>
       </c>
       <c r="K190" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L190" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.35">
@@ -7118,13 +7112,13 @@
         <v>422</v>
       </c>
       <c r="G191" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K191" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="L191" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.35">
@@ -7167,10 +7161,10 @@
         <v>20</v>
       </c>
       <c r="K193" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L193" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.35">
@@ -7193,10 +7187,10 @@
         <v>20</v>
       </c>
       <c r="K194" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L194" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.35">
@@ -7219,10 +7213,10 @@
         <v>20</v>
       </c>
       <c r="K195" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L195" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.35">
@@ -7245,10 +7239,10 @@
         <v>20</v>
       </c>
       <c r="K196" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L196" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.35">
@@ -7274,10 +7268,10 @@
         <v>22</v>
       </c>
       <c r="K197" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L197" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.35">
@@ -7300,10 +7294,10 @@
         <v>20</v>
       </c>
       <c r="K198" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L198" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.35">
@@ -7346,10 +7340,10 @@
         <v>20</v>
       </c>
       <c r="K200" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="L200" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.35">
@@ -7375,10 +7369,10 @@
         <v>22</v>
       </c>
       <c r="K201" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="L201" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.35">
@@ -7398,13 +7392,13 @@
         <v>431</v>
       </c>
       <c r="G202" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K202" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L202" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -7432,184 +7426,184 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>448</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>449</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>451</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>452</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>456</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>458</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>459</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>460</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>462</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>463</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>465</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>466</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>468</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>469</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>473</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>474</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>476</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>477</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>479</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>480</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>482</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>483</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>485</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>486</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -7617,13 +7611,13 @@
         <v>44</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>43</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>